<commit_message>
Similarity classifier added. Documentation almost done.
</commit_message>
<xml_diff>
--- a/Documentation/Classification_method_comparison.xlsx
+++ b/Documentation/Classification_method_comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/43f65f5b78f39d56/Kursseja/Fuzzy_data_analysis/Practical_assignment/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Onedrive\Kursseja\Fuzzy_data_analysis\Practical_assignment\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{F4E7AA41-77F6-4959-82F0-E76B4FC4E11E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{92CC1F31-41BA-4B6F-AA50-2D37C947CE21}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{F4E7AA41-77F6-4959-82F0-E76B4FC4E11E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{2F26D5E3-5918-43AD-BCB7-5A954A8E2587}"/>
   <bookViews>
-    <workbookView xWindow="11550" yWindow="1740" windowWidth="23625" windowHeight="15435" xr2:uid="{369BD34F-5522-4FC2-9DF0-91A1E64395E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{369BD34F-5522-4FC2-9DF0-91A1E64395E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Training set</t>
   </si>
@@ -88,6 +88,24 @@
   </si>
   <si>
     <t>Classification method</t>
+  </si>
+  <si>
+    <t>Similarity classifier</t>
+  </si>
+  <si>
+    <t>PCA &amp; Similarity classifier</t>
+  </si>
+  <si>
+    <t>PCA &amp; Similarity classifier WITH 25 columns of data</t>
+  </si>
+  <si>
+    <t>FPCA &amp; Similarity classifier</t>
+  </si>
+  <si>
+    <t>FPCA &amp; Similarity classifier WITH 25 columns of data</t>
+  </si>
+  <si>
+    <t>Simple linear regression</t>
   </si>
 </sst>
 </file>
@@ -95,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -106,26 +124,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +168,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -255,8 +279,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -266,32 +302,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <font>
         <b val="0"/>
@@ -303,10 +334,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -315,8 +346,8 @@
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -329,12 +360,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -348,10 +373,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -360,8 +385,8 @@
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -374,12 +399,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -393,10 +412,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -405,8 +424,8 @@
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -419,12 +438,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -438,10 +451,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -450,8 +463,8 @@
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -464,12 +477,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -483,10 +490,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -495,8 +502,8 @@
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -509,12 +516,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -528,10 +529,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -540,8 +541,8 @@
           <bgColor rgb="FFDEEAF6"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -554,12 +555,6 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -573,20 +568,20 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFDEEAF6"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -599,13 +594,20 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-        <vertical style="medium">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="medium">
-          <color indexed="64"/>
-        </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -618,10 +620,10 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="0"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
+        <name val="Open Sans"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
       <fill>
@@ -644,6 +646,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
@@ -651,15 +662,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
@@ -679,10 +681,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{40F94C72-70B5-472B-80D8-3F486AE77551}" name="Table2" displayName="Table2" ref="B3:H13" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="9">
-  <autoFilter ref="B3:H13" xr:uid="{0581BB4C-B796-44BA-A68B-AA671457793F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:H13">
-    <sortCondition descending="1" ref="G3:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{40F94C72-70B5-472B-80D8-3F486AE77551}" name="Table2" displayName="Table2" ref="B3:H19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="B3:H19" xr:uid="{0581BB4C-B796-44BA-A68B-AA671457793F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:H19">
+    <sortCondition descending="1" ref="G3:G19"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9B083B0E-0B59-42A1-9360-3226BB031EC0}" name="Classification method" dataDxfId="6"/>
@@ -994,15 +996,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A4E0A6-6174-44F6-BA58-EFA9096050D5}">
-  <dimension ref="B1:H13"/>
+  <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B2" sqref="B2:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
@@ -1011,242 +1013,440 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="4"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0.442</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.39100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0.46</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.874</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="G5" s="11">
+        <v>0.626</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.65300000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.83499999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.84</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C9" s="11">
         <v>0.93300000000000005</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D9" s="11">
         <v>0.318</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E9" s="11">
         <v>0.97099999999999997</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F9" s="11">
         <v>0.71799999999999997</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G9" s="11">
         <v>0.253</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H9" s="11">
         <v>0.876</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+    <row r="10" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C10" s="11">
         <v>0.93400000000000005</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D10" s="11">
         <v>0.32300000000000001</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E10" s="11">
         <v>0.97099999999999997</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F10" s="11">
         <v>0.72399999999999998</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G10" s="11">
         <v>0.251</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H10" s="11">
         <v>0.88500000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="5" t="s">
+    <row r="11" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C11" s="12">
         <v>0.94827479999999997</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D11" s="12">
         <v>0.30652170000000001</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E11" s="12">
         <v>0.98788920000000002</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F11" s="12">
         <v>0.76776759999999999</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G11" s="12">
         <v>0.2220934</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H11" s="12">
         <v>0.95383090000000004</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+    <row r="12" spans="2:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C12" s="11">
         <v>0.93700000000000006</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D12" s="11">
         <v>0.33300000000000002</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E12" s="11">
         <v>0.97099999999999997</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F12" s="11">
         <v>0.75</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G12" s="11">
         <v>0.21299999999999999</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H12" s="11">
         <v>0.93200000000000005</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+    <row r="13" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C13" s="11">
         <v>0.93300000000000005</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D13" s="11">
         <v>0.33500000000000002</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E13" s="11">
         <v>0.97</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F13" s="11">
         <v>0.75</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G13" s="11">
         <v>0.20200000000000001</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H13" s="11">
         <v>0.93700000000000006</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
+    <row r="14" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0.746</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0.17</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="F15" s="11">
+        <v>0.746</v>
+      </c>
+      <c r="G15" s="11">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="H15" s="11">
+        <v>0.94299999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.94615800000000005</v>
+      </c>
+      <c r="D16" s="12">
+        <v>0.158696</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0.99476699999999996</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0.75088500000000002</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.118005</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.96668299999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12">
         <v>0.75693010000000005</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G17" s="12">
         <v>9.1910699999999998E-2</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H17" s="12">
         <v>0.9836876</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
+    <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C18" s="12">
         <v>0.94562060000000003</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D18" s="12">
         <v>0.13913039999999999</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E18" s="12">
         <v>0.99540390000000001</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F18" s="12">
         <v>0.74837810000000005</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G18" s="12">
         <v>2.4644820000000001E-2</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H18" s="12">
         <v>0.99151557000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
+    <row r="19" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="11">
         <v>0.94189999999999996</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G19" s="11">
         <v>0</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H19" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="2:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:G13">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="G9:G10 G6">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F19">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G19">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H19">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>